<commit_message>
Data drive test case 1
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B103_Selenium\workspace2\b103afw\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\git\b103afw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95450FC7-720F-4BD4-8700-9A6160BB7071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47DFF5B-CB95-48FC-9D71-1EE0DC4DC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>bhanu</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
   </si>
 </sst>
 </file>
@@ -350,7 +360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -369,4 +379,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE312FB9-227E-477B-840D-EC3FC65FFEB0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>